<commit_message>
Update Phân tích điểm
</commit_message>
<xml_diff>
--- a/Data science starter/K18Mark.xlsx
+++ b/Data science starter/K18Mark.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52AB80D-CF5E-49C6-AC77-077DF5B6C86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Khoa CNTT" sheetId="1" r:id="rId1"/>
@@ -3283,15 +3284,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3398,8 +3399,8 @@
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -3423,15 +3424,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Comma 2" xfId="3"/>
-    <cellStyle name="Comma 3" xfId="2"/>
-    <cellStyle name="Excel Built-in Normal" xfId="4"/>
+    <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5"/>
-    <cellStyle name="Normal 3" xfId="6"/>
-    <cellStyle name="Normal 4" xfId="7"/>
-    <cellStyle name="Normal 5" xfId="8"/>
-    <cellStyle name="Normal 6" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 5" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 6" xfId="1" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3708,22 +3709,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G328"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.625" customWidth="1"/>
+    <col min="2" max="2" width="21.875" customWidth="1"/>
+    <col min="3" max="3" width="13.625" customWidth="1"/>
+    <col min="7" max="7" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1079</v>
       </c>
@@ -3746,7 +3747,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3769,7 +3770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -3792,7 +3793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -3815,7 +3816,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -3838,7 +3839,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -3861,7 +3862,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -3884,7 +3885,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -3907,7 +3908,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
@@ -3930,7 +3931,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
@@ -3953,7 +3954,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
@@ -3976,7 +3977,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>49</v>
       </c>
@@ -3999,7 +4000,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>54</v>
       </c>
@@ -4022,7 +4023,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>59</v>
       </c>
@@ -4045,7 +4046,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>64</v>
       </c>
@@ -4068,7 +4069,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>67</v>
       </c>
@@ -4091,7 +4092,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>72</v>
       </c>
@@ -4114,7 +4115,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>75</v>
       </c>
@@ -4137,7 +4138,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>80</v>
       </c>
@@ -4160,7 +4161,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>85</v>
       </c>
@@ -4183,7 +4184,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>89</v>
       </c>
@@ -4206,7 +4207,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>93</v>
       </c>
@@ -4229,7 +4230,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>98</v>
       </c>
@@ -4252,7 +4253,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>102</v>
       </c>
@@ -4275,7 +4276,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>106</v>
       </c>
@@ -4298,7 +4299,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>111</v>
       </c>
@@ -4321,7 +4322,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>115</v>
       </c>
@@ -4344,7 +4345,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>119</v>
       </c>
@@ -4367,7 +4368,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>123</v>
       </c>
@@ -4390,7 +4391,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>127</v>
       </c>
@@ -4413,7 +4414,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>132</v>
       </c>
@@ -4436,7 +4437,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>137</v>
       </c>
@@ -4459,7 +4460,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>141</v>
       </c>
@@ -4482,7 +4483,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>145</v>
       </c>
@@ -4505,7 +4506,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>149</v>
       </c>
@@ -4528,7 +4529,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>152</v>
       </c>
@@ -4551,7 +4552,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>156</v>
       </c>
@@ -4574,7 +4575,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>161</v>
       </c>
@@ -4597,7 +4598,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>165</v>
       </c>
@@ -4620,7 +4621,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>171</v>
       </c>
@@ -4643,7 +4644,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>174</v>
       </c>
@@ -4666,7 +4667,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>177</v>
       </c>
@@ -4689,7 +4690,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>181</v>
       </c>
@@ -4712,7 +4713,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>186</v>
       </c>
@@ -4735,7 +4736,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>189</v>
       </c>
@@ -4758,7 +4759,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>193</v>
       </c>
@@ -4781,7 +4782,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>197</v>
       </c>
@@ -4804,7 +4805,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>201</v>
       </c>
@@ -4827,7 +4828,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>205</v>
       </c>
@@ -4850,7 +4851,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>208</v>
       </c>
@@ -4873,7 +4874,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>211</v>
       </c>
@@ -4896,7 +4897,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>214</v>
       </c>
@@ -4919,7 +4920,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>218</v>
       </c>
@@ -4942,7 +4943,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>221</v>
       </c>
@@ -4965,7 +4966,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>225</v>
       </c>
@@ -4988,7 +4989,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>229</v>
       </c>
@@ -5011,7 +5012,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>233</v>
       </c>
@@ -5034,7 +5035,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>237</v>
       </c>
@@ -5057,7 +5058,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>239</v>
       </c>
@@ -5080,7 +5081,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>243</v>
       </c>
@@ -5103,7 +5104,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>247</v>
       </c>
@@ -5126,7 +5127,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>252</v>
       </c>
@@ -5149,7 +5150,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>256</v>
       </c>
@@ -5172,7 +5173,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>259</v>
       </c>
@@ -5195,7 +5196,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>263</v>
       </c>
@@ -5218,7 +5219,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>266</v>
       </c>
@@ -5241,7 +5242,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>271</v>
       </c>
@@ -5264,7 +5265,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>274</v>
       </c>
@@ -5287,7 +5288,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>279</v>
       </c>
@@ -5310,7 +5311,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>284</v>
       </c>
@@ -5333,7 +5334,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>289</v>
       </c>
@@ -5356,7 +5357,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>293</v>
       </c>
@@ -5379,7 +5380,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>297</v>
       </c>
@@ -5402,7 +5403,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>301</v>
       </c>
@@ -5425,7 +5426,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>305</v>
       </c>
@@ -5448,7 +5449,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>308</v>
       </c>
@@ -5471,7 +5472,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>312</v>
       </c>
@@ -5494,7 +5495,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>317</v>
       </c>
@@ -5517,7 +5518,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>322</v>
       </c>
@@ -5540,7 +5541,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>326</v>
       </c>
@@ -5563,7 +5564,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>331</v>
       </c>
@@ -5586,7 +5587,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>333</v>
       </c>
@@ -5609,7 +5610,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>337</v>
       </c>
@@ -5632,7 +5633,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>341</v>
       </c>
@@ -5655,7 +5656,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>346</v>
       </c>
@@ -5678,7 +5679,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>350</v>
       </c>
@@ -5701,7 +5702,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>352</v>
       </c>
@@ -5724,7 +5725,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>355</v>
       </c>
@@ -5747,7 +5748,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>359</v>
       </c>
@@ -5770,7 +5771,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>362</v>
       </c>
@@ -5793,7 +5794,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>365</v>
       </c>
@@ -5816,7 +5817,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>370</v>
       </c>
@@ -5839,7 +5840,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>373</v>
       </c>
@@ -5862,7 +5863,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>376</v>
       </c>
@@ -5885,7 +5886,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>381</v>
       </c>
@@ -5908,7 +5909,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>383</v>
       </c>
@@ -5931,7 +5932,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>386</v>
       </c>
@@ -5954,7 +5955,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>389</v>
       </c>
@@ -5977,7 +5978,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>392</v>
       </c>
@@ -6000,7 +6001,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>396</v>
       </c>
@@ -6023,7 +6024,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>398</v>
       </c>
@@ -6046,7 +6047,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>401</v>
       </c>
@@ -6069,7 +6070,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>404</v>
       </c>
@@ -6092,7 +6093,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>409</v>
       </c>
@@ -6115,7 +6116,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>411</v>
       </c>
@@ -6138,7 +6139,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>415</v>
       </c>
@@ -6161,7 +6162,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>418</v>
       </c>
@@ -6184,7 +6185,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>422</v>
       </c>
@@ -6207,7 +6208,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>425</v>
       </c>
@@ -6230,7 +6231,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>428</v>
       </c>
@@ -6253,7 +6254,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>432</v>
       </c>
@@ -6276,7 +6277,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>437</v>
       </c>
@@ -6299,7 +6300,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>441</v>
       </c>
@@ -6322,7 +6323,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>445</v>
       </c>
@@ -6345,7 +6346,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>448</v>
       </c>
@@ -6368,7 +6369,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>453</v>
       </c>
@@ -6391,7 +6392,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>457</v>
       </c>
@@ -6414,7 +6415,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>461</v>
       </c>
@@ -6437,7 +6438,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>464</v>
       </c>
@@ -6460,7 +6461,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>468</v>
       </c>
@@ -6483,7 +6484,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>470</v>
       </c>
@@ -6506,7 +6507,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>474</v>
       </c>
@@ -6529,7 +6530,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>477</v>
       </c>
@@ -6552,7 +6553,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>480</v>
       </c>
@@ -6575,7 +6576,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>485</v>
       </c>
@@ -6598,7 +6599,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>490</v>
       </c>
@@ -6621,7 +6622,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>493</v>
       </c>
@@ -6644,7 +6645,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>496</v>
       </c>
@@ -6667,7 +6668,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>499</v>
       </c>
@@ -6690,7 +6691,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>501</v>
       </c>
@@ -6713,7 +6714,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>503</v>
       </c>
@@ -6736,7 +6737,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>506</v>
       </c>
@@ -6759,7 +6760,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>510</v>
       </c>
@@ -6782,7 +6783,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>514</v>
       </c>
@@ -6805,7 +6806,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>518</v>
       </c>
@@ -6828,7 +6829,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>520</v>
       </c>
@@ -6851,7 +6852,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>525</v>
       </c>
@@ -6874,7 +6875,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>529</v>
       </c>
@@ -6897,7 +6898,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>533</v>
       </c>
@@ -6920,7 +6921,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>537</v>
       </c>
@@ -6943,7 +6944,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>540</v>
       </c>
@@ -6966,7 +6967,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>543</v>
       </c>
@@ -6989,7 +6990,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>548</v>
       </c>
@@ -7012,7 +7013,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>551</v>
       </c>
@@ -7035,7 +7036,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>554</v>
       </c>
@@ -7058,7 +7059,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>557</v>
       </c>
@@ -7081,7 +7082,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>561</v>
       </c>
@@ -7104,7 +7105,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>565</v>
       </c>
@@ -7127,7 +7128,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>568</v>
       </c>
@@ -7150,7 +7151,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>573</v>
       </c>
@@ -7173,7 +7174,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>577</v>
       </c>
@@ -7196,7 +7197,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>581</v>
       </c>
@@ -7219,7 +7220,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>585</v>
       </c>
@@ -7242,7 +7243,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>589</v>
       </c>
@@ -7265,7 +7266,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>591</v>
       </c>
@@ -7288,7 +7289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>593</v>
       </c>
@@ -7311,7 +7312,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>596</v>
       </c>
@@ -7334,7 +7335,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>600</v>
       </c>
@@ -7357,7 +7358,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>603</v>
       </c>
@@ -7380,7 +7381,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>605</v>
       </c>
@@ -7403,7 +7404,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>607</v>
       </c>
@@ -7426,7 +7427,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>609</v>
       </c>
@@ -7449,7 +7450,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>612</v>
       </c>
@@ -7472,7 +7473,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>614</v>
       </c>
@@ -7495,7 +7496,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>616</v>
       </c>
@@ -7518,7 +7519,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>617</v>
       </c>
@@ -7541,7 +7542,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>621</v>
       </c>
@@ -7564,7 +7565,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>625</v>
       </c>
@@ -7587,7 +7588,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>627</v>
       </c>
@@ -7610,7 +7611,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>629</v>
       </c>
@@ -7633,7 +7634,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>633</v>
       </c>
@@ -7656,7 +7657,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
         <v>634</v>
       </c>
@@ -7679,7 +7680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>636</v>
       </c>
@@ -7702,7 +7703,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>639</v>
       </c>
@@ -7725,7 +7726,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>641</v>
       </c>
@@ -7748,7 +7749,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>642</v>
       </c>
@@ -7771,7 +7772,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>646</v>
       </c>
@@ -7794,7 +7795,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>650</v>
       </c>
@@ -7817,7 +7818,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
         <v>654</v>
       </c>
@@ -7840,7 +7841,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
         <v>657</v>
       </c>
@@ -7863,7 +7864,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>659</v>
       </c>
@@ -7886,7 +7887,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>662</v>
       </c>
@@ -7909,7 +7910,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>664</v>
       </c>
@@ -7932,7 +7933,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>666</v>
       </c>
@@ -7955,7 +7956,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>669</v>
       </c>
@@ -7978,7 +7979,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
         <v>674</v>
       </c>
@@ -8001,7 +8002,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>677</v>
       </c>
@@ -8024,7 +8025,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
         <v>680</v>
       </c>
@@ -8047,7 +8048,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
         <v>683</v>
       </c>
@@ -8070,7 +8071,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
         <v>687</v>
       </c>
@@ -8093,7 +8094,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
         <v>689</v>
       </c>
@@ -8116,7 +8117,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
         <v>693</v>
       </c>
@@ -8139,7 +8140,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>697</v>
       </c>
@@ -8162,7 +8163,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
         <v>699</v>
       </c>
@@ -8185,7 +8186,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
         <v>703</v>
       </c>
@@ -8208,7 +8209,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
         <v>705</v>
       </c>
@@ -8231,7 +8232,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>708</v>
       </c>
@@ -8254,7 +8255,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
         <v>710</v>
       </c>
@@ -8277,7 +8278,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
         <v>713</v>
       </c>
@@ -8300,7 +8301,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
         <v>716</v>
       </c>
@@ -8323,7 +8324,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
         <v>719</v>
       </c>
@@ -8346,7 +8347,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
         <v>722</v>
       </c>
@@ -8369,7 +8370,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>724</v>
       </c>
@@ -8392,7 +8393,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
         <v>727</v>
       </c>
@@ -8415,7 +8416,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
         <v>731</v>
       </c>
@@ -8438,7 +8439,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
         <v>734</v>
       </c>
@@ -8461,7 +8462,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>736</v>
       </c>
@@ -8484,7 +8485,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
         <v>739</v>
       </c>
@@ -8507,7 +8508,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
         <v>742</v>
       </c>
@@ -8530,7 +8531,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
         <v>745</v>
       </c>
@@ -8553,7 +8554,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
         <v>747</v>
       </c>
@@ -8576,7 +8577,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
         <v>751</v>
       </c>
@@ -8599,7 +8600,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
         <v>754</v>
       </c>
@@ -8622,7 +8623,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
         <v>757</v>
       </c>
@@ -8645,7 +8646,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
         <v>759</v>
       </c>
@@ -8668,7 +8669,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
         <v>763</v>
       </c>
@@ -8691,7 +8692,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
         <v>767</v>
       </c>
@@ -8714,7 +8715,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
         <v>771</v>
       </c>
@@ -8737,7 +8738,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
         <v>774</v>
       </c>
@@ -8760,7 +8761,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
         <v>778</v>
       </c>
@@ -8783,7 +8784,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
         <v>781</v>
       </c>
@@ -8806,7 +8807,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
         <v>784</v>
       </c>
@@ -8829,7 +8830,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
         <v>786</v>
       </c>
@@ -8852,7 +8853,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
         <v>788</v>
       </c>
@@ -8875,7 +8876,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
         <v>792</v>
       </c>
@@ -8898,7 +8899,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
         <v>795</v>
       </c>
@@ -8921,7 +8922,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
         <v>798</v>
       </c>
@@ -8944,7 +8945,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
         <v>802</v>
       </c>
@@ -8967,7 +8968,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
         <v>805</v>
       </c>
@@ -8990,7 +8991,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
         <v>808</v>
       </c>
@@ -9013,7 +9014,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
         <v>811</v>
       </c>
@@ -9036,7 +9037,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
         <v>814</v>
       </c>
@@ -9059,7 +9060,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
         <v>816</v>
       </c>
@@ -9082,7 +9083,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
         <v>817</v>
       </c>
@@ -9105,7 +9106,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
         <v>820</v>
       </c>
@@ -9128,7 +9129,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
         <v>823</v>
       </c>
@@ -9151,7 +9152,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
         <v>826</v>
       </c>
@@ -9174,7 +9175,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
         <v>829</v>
       </c>
@@ -9197,7 +9198,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
         <v>830</v>
       </c>
@@ -9220,7 +9221,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
         <v>832</v>
       </c>
@@ -9243,7 +9244,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
         <v>834</v>
       </c>
@@ -9266,7 +9267,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
         <v>836</v>
       </c>
@@ -9289,7 +9290,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="s">
         <v>838</v>
       </c>
@@ -9312,7 +9313,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="s">
         <v>841</v>
       </c>
@@ -9335,7 +9336,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="s">
         <v>845</v>
       </c>
@@ -9358,7 +9359,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="s">
         <v>847</v>
       </c>
@@ -9381,7 +9382,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="s">
         <v>850</v>
       </c>
@@ -9404,7 +9405,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
         <v>851</v>
       </c>
@@ -9427,7 +9428,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
         <v>853</v>
       </c>
@@ -9450,7 +9451,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="s">
         <v>855</v>
       </c>
@@ -9473,7 +9474,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="s">
         <v>858</v>
       </c>
@@ -9496,7 +9497,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
         <v>859</v>
       </c>
@@ -9519,7 +9520,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
         <v>863</v>
       </c>
@@ -9542,7 +9543,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
         <v>865</v>
       </c>
@@ -9565,7 +9566,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A255" s="3" t="s">
         <v>869</v>
       </c>
@@ -9588,7 +9589,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A256" s="3" t="s">
         <v>872</v>
       </c>
@@ -9611,7 +9612,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
         <v>874</v>
       </c>
@@ -9634,7 +9635,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="s">
         <v>876</v>
       </c>
@@ -9657,7 +9658,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="s">
         <v>879</v>
       </c>
@@ -9680,7 +9681,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A260" s="3" t="s">
         <v>883</v>
       </c>
@@ -9703,7 +9704,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A261" s="3" t="s">
         <v>885</v>
       </c>
@@ -9726,7 +9727,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="s">
         <v>889</v>
       </c>
@@ -9749,7 +9750,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A263" s="3" t="s">
         <v>893</v>
       </c>
@@ -9772,7 +9773,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A264" s="3" t="s">
         <v>898</v>
       </c>
@@ -9795,7 +9796,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A265" s="3" t="s">
         <v>902</v>
       </c>
@@ -9818,7 +9819,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="s">
         <v>905</v>
       </c>
@@ -9841,7 +9842,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A267" s="3" t="s">
         <v>909</v>
       </c>
@@ -9864,7 +9865,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A268" s="3" t="s">
         <v>910</v>
       </c>
@@ -9887,7 +9888,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A269" s="3" t="s">
         <v>912</v>
       </c>
@@ -9910,7 +9911,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A270" s="3" t="s">
         <v>916</v>
       </c>
@@ -9933,7 +9934,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A271" s="3" t="s">
         <v>919</v>
       </c>
@@ -9956,7 +9957,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A272" s="3" t="s">
         <v>923</v>
       </c>
@@ -9979,7 +9980,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A273" s="3" t="s">
         <v>925</v>
       </c>
@@ -10002,7 +10003,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A274" s="3" t="s">
         <v>927</v>
       </c>
@@ -10025,7 +10026,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A275" s="3" t="s">
         <v>930</v>
       </c>
@@ -10048,7 +10049,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A276" s="3" t="s">
         <v>933</v>
       </c>
@@ -10071,7 +10072,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="s">
         <v>936</v>
       </c>
@@ -10094,7 +10095,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A278" s="3" t="s">
         <v>940</v>
       </c>
@@ -10117,7 +10118,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A279" s="3" t="s">
         <v>943</v>
       </c>
@@ -10140,7 +10141,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A280" s="3" t="s">
         <v>947</v>
       </c>
@@ -10163,7 +10164,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A281" s="3" t="s">
         <v>950</v>
       </c>
@@ -10186,7 +10187,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A282" s="3" t="s">
         <v>953</v>
       </c>
@@ -10209,7 +10210,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A283" s="3" t="s">
         <v>957</v>
       </c>
@@ -10232,7 +10233,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A284" s="3" t="s">
         <v>960</v>
       </c>
@@ -10255,7 +10256,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A285" s="3" t="s">
         <v>961</v>
       </c>
@@ -10278,7 +10279,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A286" s="3" t="s">
         <v>964</v>
       </c>
@@ -10301,7 +10302,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A287" s="3" t="s">
         <v>965</v>
       </c>
@@ -10324,7 +10325,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A288" s="3" t="s">
         <v>968</v>
       </c>
@@ -10347,7 +10348,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A289" s="3" t="s">
         <v>970</v>
       </c>
@@ -10370,7 +10371,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A290" s="3" t="s">
         <v>973</v>
       </c>
@@ -10393,7 +10394,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A291" s="3" t="s">
         <v>975</v>
       </c>
@@ -10416,7 +10417,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A292" s="3" t="s">
         <v>979</v>
       </c>
@@ -10439,7 +10440,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A293" s="3" t="s">
         <v>983</v>
       </c>
@@ -10462,7 +10463,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A294" s="3" t="s">
         <v>986</v>
       </c>
@@ -10485,7 +10486,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A295" s="3" t="s">
         <v>987</v>
       </c>
@@ -10508,7 +10509,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A296" s="3" t="s">
         <v>991</v>
       </c>
@@ -10531,7 +10532,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A297" s="3" t="s">
         <v>995</v>
       </c>
@@ -10554,7 +10555,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A298" s="3" t="s">
         <v>998</v>
       </c>
@@ -10577,7 +10578,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A299" s="3" t="s">
         <v>1001</v>
       </c>
@@ -10600,7 +10601,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A300" s="3" t="s">
         <v>1004</v>
       </c>
@@ -10623,7 +10624,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A301" s="3" t="s">
         <v>1006</v>
       </c>
@@ -10646,7 +10647,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A302" s="3" t="s">
         <v>1008</v>
       </c>
@@ -10669,7 +10670,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A303" s="3" t="s">
         <v>1010</v>
       </c>
@@ -10692,7 +10693,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A304" s="3" t="s">
         <v>1013</v>
       </c>
@@ -10715,7 +10716,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A305" s="3" t="s">
         <v>1015</v>
       </c>
@@ -10738,7 +10739,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A306" s="3" t="s">
         <v>1017</v>
       </c>
@@ -10761,7 +10762,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A307" s="3" t="s">
         <v>1019</v>
       </c>
@@ -10784,7 +10785,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A308" s="3" t="s">
         <v>1023</v>
       </c>
@@ -10807,7 +10808,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A309" s="3" t="s">
         <v>1025</v>
       </c>
@@ -10830,7 +10831,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A310" s="3" t="s">
         <v>1028</v>
       </c>
@@ -10853,7 +10854,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A311" s="3" t="s">
         <v>1031</v>
       </c>
@@ -10876,7 +10877,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A312" s="3" t="s">
         <v>1035</v>
       </c>
@@ -10899,7 +10900,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A313" s="3" t="s">
         <v>1037</v>
       </c>
@@ -10922,7 +10923,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A314" s="3" t="s">
         <v>1039</v>
       </c>
@@ -10945,7 +10946,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A315" s="3" t="s">
         <v>1043</v>
       </c>
@@ -10968,7 +10969,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A316" s="3" t="s">
         <v>1046</v>
       </c>
@@ -10991,7 +10992,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A317" s="3" t="s">
         <v>1049</v>
       </c>
@@ -11014,7 +11015,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A318" s="3" t="s">
         <v>1052</v>
       </c>
@@ -11037,7 +11038,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A319" s="3" t="s">
         <v>1055</v>
       </c>
@@ -11060,7 +11061,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A320" s="3" t="s">
         <v>1056</v>
       </c>
@@ -11083,7 +11084,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A321" s="3" t="s">
         <v>1058</v>
       </c>
@@ -11106,7 +11107,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A322" s="3" t="s">
         <v>1061</v>
       </c>
@@ -11129,7 +11130,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A323" s="3" t="s">
         <v>1063</v>
       </c>
@@ -11152,7 +11153,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A324" s="3" t="s">
         <v>1065</v>
       </c>
@@ -11175,7 +11176,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A325" s="3" t="s">
         <v>1068</v>
       </c>
@@ -11198,7 +11199,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A326" s="3" t="s">
         <v>1072</v>
       </c>
@@ -11221,7 +11222,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A327" s="3" t="s">
         <v>1074</v>
       </c>
@@ -11244,7 +11245,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A328" s="3" t="s">
         <v>1076</v>
       </c>
@@ -11273,16 +11274,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="P109" sqref="P109"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1079</v>
       </c>
@@ -11305,7 +11306,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>54</v>
       </c>
@@ -11328,7 +11329,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>59</v>
       </c>
@@ -11351,7 +11352,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>64</v>
       </c>
@@ -11374,7 +11375,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>67</v>
       </c>
@@ -11397,7 +11398,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
@@ -11420,7 +11421,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>75</v>
       </c>
@@ -11443,7 +11444,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>80</v>
       </c>
@@ -11466,7 +11467,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>85</v>
       </c>
@@ -11489,7 +11490,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>89</v>
       </c>
@@ -11512,7 +11513,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>93</v>
       </c>
@@ -11535,7 +11536,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>98</v>
       </c>
@@ -11558,7 +11559,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>102</v>
       </c>
@@ -11581,7 +11582,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>106</v>
       </c>
@@ -11604,7 +11605,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>111</v>
       </c>
@@ -11627,7 +11628,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>115</v>
       </c>
@@ -11650,7 +11651,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>119</v>
       </c>
@@ -11673,7 +11674,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>123</v>
       </c>
@@ -11696,7 +11697,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>127</v>
       </c>
@@ -11719,7 +11720,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>132</v>
       </c>
@@ -11742,7 +11743,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>137</v>
       </c>
@@ -11765,7 +11766,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>141</v>
       </c>
@@ -11788,7 +11789,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>145</v>
       </c>
@@ -11811,7 +11812,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>149</v>
       </c>
@@ -11834,7 +11835,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>152</v>
       </c>
@@ -11857,7 +11858,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>156</v>
       </c>
@@ -11880,7 +11881,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>161</v>
       </c>
@@ -11903,7 +11904,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>165</v>
       </c>
@@ -11926,7 +11927,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>171</v>
       </c>
@@ -11949,7 +11950,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>174</v>
       </c>
@@ -11972,7 +11973,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>177</v>
       </c>
@@ -11995,7 +11996,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>181</v>
       </c>
@@ -12018,7 +12019,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>186</v>
       </c>
@@ -12041,7 +12042,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>189</v>
       </c>
@@ -12064,7 +12065,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>193</v>
       </c>
@@ -12087,7 +12088,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>197</v>
       </c>
@@ -12110,7 +12111,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>201</v>
       </c>
@@ -12133,7 +12134,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>205</v>
       </c>
@@ -12156,7 +12157,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>208</v>
       </c>
@@ -12179,7 +12180,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>211</v>
       </c>
@@ -12202,7 +12203,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>214</v>
       </c>
@@ -12225,7 +12226,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>218</v>
       </c>
@@ -12248,7 +12249,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>221</v>
       </c>
@@ -12271,7 +12272,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>225</v>
       </c>
@@ -12294,7 +12295,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>229</v>
       </c>
@@ -12317,7 +12318,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>233</v>
       </c>
@@ -12340,7 +12341,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>237</v>
       </c>
@@ -12363,7 +12364,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>239</v>
       </c>
@@ -12386,7 +12387,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>243</v>
       </c>
@@ -12409,7 +12410,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>247</v>
       </c>
@@ -12432,7 +12433,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>252</v>
       </c>
@@ -12455,7 +12456,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>256</v>
       </c>
@@ -12478,7 +12479,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>259</v>
       </c>
@@ -12501,7 +12502,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>263</v>
       </c>
@@ -12524,7 +12525,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>266</v>
       </c>
@@ -12547,7 +12548,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>271</v>
       </c>
@@ -12570,7 +12571,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>274</v>
       </c>
@@ -12593,7 +12594,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>279</v>
       </c>
@@ -12616,7 +12617,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>284</v>
       </c>
@@ -12639,7 +12640,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>289</v>
       </c>
@@ -12662,7 +12663,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>293</v>
       </c>
@@ -12685,7 +12686,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>297</v>
       </c>
@@ -12708,7 +12709,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>301</v>
       </c>
@@ -12731,7 +12732,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>305</v>
       </c>
@@ -12754,7 +12755,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>308</v>
       </c>
@@ -12777,7 +12778,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>312</v>
       </c>
@@ -12800,7 +12801,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>317</v>
       </c>
@@ -12823,7 +12824,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>322</v>
       </c>
@@ -12846,7 +12847,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>326</v>
       </c>
@@ -12869,7 +12870,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>331</v>
       </c>
@@ -12892,7 +12893,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>333</v>
       </c>
@@ -12915,7 +12916,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>337</v>
       </c>
@@ -12938,7 +12939,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>341</v>
       </c>
@@ -12961,7 +12962,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>346</v>
       </c>
@@ -12984,7 +12985,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>350</v>
       </c>
@@ -13007,7 +13008,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>352</v>
       </c>
@@ -13030,7 +13031,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>355</v>
       </c>
@@ -13053,7 +13054,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>359</v>
       </c>
@@ -13076,7 +13077,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>362</v>
       </c>
@@ -13099,7 +13100,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>365</v>
       </c>
@@ -13122,7 +13123,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>370</v>
       </c>
@@ -13145,7 +13146,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>373</v>
       </c>
@@ -13168,7 +13169,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>376</v>
       </c>
@@ -13191,7 +13192,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>381</v>
       </c>
@@ -13214,7 +13215,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>383</v>
       </c>
@@ -13237,7 +13238,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>386</v>
       </c>
@@ -13260,7 +13261,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>389</v>
       </c>
@@ -13283,7 +13284,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>392</v>
       </c>
@@ -13306,7 +13307,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>396</v>
       </c>
@@ -13329,7 +13330,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>398</v>
       </c>
@@ -13352,7 +13353,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>401</v>
       </c>
@@ -13375,7 +13376,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>404</v>
       </c>
@@ -13398,7 +13399,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>409</v>
       </c>
@@ -13421,7 +13422,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>411</v>
       </c>
@@ -13444,7 +13445,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>415</v>
       </c>
@@ -13467,7 +13468,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>418</v>
       </c>
@@ -13490,7 +13491,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>422</v>
       </c>
@@ -13513,7 +13514,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>425</v>
       </c>
@@ -13536,7 +13537,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>428</v>
       </c>
@@ -13559,7 +13560,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>432</v>
       </c>
@@ -13582,7 +13583,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>437</v>
       </c>
@@ -13605,7 +13606,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>441</v>
       </c>
@@ -13628,7 +13629,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>445</v>
       </c>
@@ -13651,7 +13652,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>448</v>
       </c>
@@ -13674,7 +13675,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>453</v>
       </c>
@@ -13697,7 +13698,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>457</v>
       </c>
@@ -13720,7 +13721,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>461</v>
       </c>
@@ -13743,7 +13744,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>464</v>
       </c>
@@ -13766,7 +13767,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>468</v>
       </c>
@@ -13789,7 +13790,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>470</v>
       </c>
@@ -13812,7 +13813,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>474</v>
       </c>
@@ -13835,7 +13836,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>477</v>
       </c>
@@ -13858,7 +13859,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>480</v>
       </c>
@@ -13881,7 +13882,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>485</v>
       </c>
@@ -13904,7 +13905,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>490</v>
       </c>
@@ -13927,7 +13928,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>493</v>
       </c>
@@ -13950,7 +13951,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>496</v>
       </c>
@@ -13973,7 +13974,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>499</v>
       </c>
@@ -13996,7 +13997,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>501</v>
       </c>
@@ -14019,7 +14020,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>503</v>
       </c>
@@ -14042,7 +14043,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>506</v>
       </c>
@@ -14065,7 +14066,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>510</v>
       </c>
@@ -14088,7 +14089,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>514</v>
       </c>
@@ -14111,7 +14112,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>518</v>
       </c>
@@ -14134,7 +14135,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>520</v>
       </c>
@@ -14157,7 +14158,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>525</v>
       </c>
@@ -14180,7 +14181,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>529</v>
       </c>
@@ -14203,7 +14204,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>533</v>
       </c>
@@ -14226,7 +14227,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>537</v>
       </c>
@@ -14249,7 +14250,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>540</v>
       </c>
@@ -14272,7 +14273,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>543</v>
       </c>
@@ -14295,7 +14296,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>548</v>
       </c>
@@ -14318,7 +14319,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>551</v>
       </c>
@@ -14341,7 +14342,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>554</v>
       </c>
@@ -14364,7 +14365,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>557</v>
       </c>
@@ -14387,7 +14388,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>561</v>
       </c>
@@ -14410,7 +14411,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>565</v>
       </c>
@@ -14433,7 +14434,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>568</v>
       </c>
@@ -14456,7 +14457,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>573</v>
       </c>
@@ -14479,7 +14480,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>577</v>
       </c>
@@ -14502,7 +14503,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>581</v>
       </c>
@@ -14525,7 +14526,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>585</v>
       </c>
@@ -14548,7 +14549,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>589</v>
       </c>
@@ -14571,7 +14572,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>591</v>
       </c>
@@ -14594,7 +14595,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>593</v>
       </c>
@@ -14617,7 +14618,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>596</v>
       </c>
@@ -14640,7 +14641,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>600</v>
       </c>
@@ -14663,7 +14664,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>603</v>
       </c>
@@ -14686,7 +14687,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>605</v>
       </c>
@@ -14709,7 +14710,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>607</v>
       </c>
@@ -14732,7 +14733,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>609</v>
       </c>
@@ -14755,7 +14756,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>612</v>
       </c>
@@ -14778,7 +14779,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>614</v>
       </c>
@@ -14801,7 +14802,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>616</v>
       </c>
@@ -14824,7 +14825,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>617</v>
       </c>
@@ -14847,7 +14848,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>621</v>
       </c>
@@ -14870,7 +14871,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>625</v>
       </c>
@@ -14893,7 +14894,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>627</v>
       </c>
@@ -14916,7 +14917,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>629</v>
       </c>
@@ -14939,7 +14940,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>633</v>
       </c>
@@ -14962,7 +14963,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>634</v>
       </c>
@@ -14985,7 +14986,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>636</v>
       </c>
@@ -15008,7 +15009,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>639</v>
       </c>
@@ -15031,7 +15032,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>641</v>
       </c>
@@ -15054,7 +15055,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>642</v>
       </c>
@@ -15077,7 +15078,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>646</v>
       </c>
@@ -15100,7 +15101,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>650</v>
       </c>
@@ -15123,7 +15124,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>654</v>
       </c>
@@ -15146,7 +15147,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>657</v>
       </c>
@@ -15169,7 +15170,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>659</v>
       </c>
@@ -15192,7 +15193,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>662</v>
       </c>
@@ -15215,7 +15216,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
         <v>664</v>
       </c>
@@ -15238,7 +15239,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>666</v>
       </c>
@@ -15261,7 +15262,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>669</v>
       </c>
@@ -15284,7 +15285,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>674</v>
       </c>
@@ -15307,7 +15308,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>677</v>
       </c>
@@ -15330,7 +15331,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>680</v>
       </c>
@@ -15353,7 +15354,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>683</v>
       </c>
@@ -15376,7 +15377,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
         <v>687</v>
       </c>
@@ -15399,7 +15400,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
         <v>689</v>
       </c>
@@ -15422,7 +15423,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>693</v>
       </c>
@@ -15445,7 +15446,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>697</v>
       </c>
@@ -15468,7 +15469,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>699</v>
       </c>
@@ -15491,7 +15492,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>703</v>
       </c>
@@ -15514,7 +15515,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>705</v>
       </c>
@@ -15537,7 +15538,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
         <v>708</v>
       </c>
@@ -15560,7 +15561,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>710</v>
       </c>
@@ -15583,7 +15584,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
         <v>713</v>
       </c>
@@ -15606,7 +15607,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
         <v>716</v>
       </c>
@@ -15629,7 +15630,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
         <v>719</v>
       </c>
@@ -15652,7 +15653,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
         <v>722</v>
       </c>
@@ -15675,7 +15676,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
         <v>724</v>
       </c>
@@ -15698,7 +15699,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>727</v>
       </c>
@@ -15721,7 +15722,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
         <v>731</v>
       </c>
@@ -15744,7 +15745,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
         <v>734</v>
       </c>
@@ -15767,7 +15768,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
         <v>736</v>
       </c>
@@ -15790,7 +15791,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>739</v>
       </c>
@@ -15813,7 +15814,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
         <v>742</v>
       </c>
@@ -15836,7 +15837,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
         <v>745</v>
       </c>
@@ -15859,7 +15860,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
         <v>747</v>
       </c>
@@ -15882,7 +15883,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
         <v>751</v>
       </c>
@@ -15905,7 +15906,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
         <v>754</v>
       </c>
@@ -15928,7 +15929,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>757</v>
       </c>
@@ -15951,7 +15952,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
         <v>759</v>
       </c>
@@ -15974,7 +15975,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
         <v>763</v>
       </c>
@@ -15997,7 +15998,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
         <v>767</v>
       </c>
@@ -16020,7 +16021,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>771</v>
       </c>
@@ -16043,7 +16044,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
         <v>774</v>
       </c>
@@ -16066,7 +16067,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
         <v>778</v>
       </c>
@@ -16089,7 +16090,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
         <v>781</v>
       </c>
@@ -16112,7 +16113,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
         <v>784</v>
       </c>
@@ -16135,7 +16136,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
         <v>786</v>
       </c>

</xml_diff>